<commit_message>
Update day01 and 02 Excel lesson, add new data and images
Expanded and reorganized the day01 Excel lesson with new sections, improved exercises, and clearer workflow instructions. Added new images for data entry and repository download, updated and added raw data files (PSP and distributions), and removed obsolete test data. Synchronized documentation and HTML output to reflect these changes.
</commit_message>
<xml_diff>
--- a/data/raw/PSP/PSP_NPD42_OH.xlsx
+++ b/data/raw/PSP/PSP_NPD42_OH.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohagen\Documents\GitHub\course_DigitalCompetenceInTheBiologicalSciences\data\raw\PSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EDC1D1-54D6-4D96-B081-E2ADC3DB2907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9488C2BB-F1EF-4DBE-BB0F-209DECA6398D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="318">
   <si>
     <t>X</t>
   </si>
@@ -996,6 +996,12 @@
   <si>
     <t>Height</t>
   </si>
+  <si>
+    <t>1O.4</t>
+  </si>
+  <si>
+    <t>Brossimium alicastrum (Ramon)</t>
+  </si>
 </sst>
 </file>
 
@@ -1632,7 +1638,7 @@
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1683,6 +1689,9 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - 强调文字颜色 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -7203,7 +7212,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="T3:U8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -7631,7 +7640,7 @@
   <dimension ref="A1:N704"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8842,8 +8851,36 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
+      <c r="A55">
+        <v>1234</v>
+      </c>
+      <c r="B55" t="s">
+        <v>317</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55" t="s">
+        <v>273</v>
+      </c>
+      <c r="F55" t="s">
+        <v>272</v>
+      </c>
+      <c r="G55" t="s">
+        <v>272</v>
+      </c>
+      <c r="H55" s="22">
+        <v>-88.336830000000006</v>
+      </c>
+      <c r="I55" s="22">
+        <v>18.03153</v>
+      </c>
+      <c r="J55">
+        <v>57.3</v>
+      </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H56" s="22"/>
@@ -8893,8 +8930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI900"/>
   <sheetViews>
-    <sheetView topLeftCell="Q8" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9125,9 +9162,9 @@
         <f t="array" ref="AC9">INDEX($O$21:$O$900, MATCH(0, COUNTIF($AC$2:AC8, $O$21:$O$900), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="AG9" t="e">
+      <c r="AG9" t="str">
         <f t="array" ref="AG9">INDEX($P$21:$P$900, MATCH(0, COUNTIF($AG$2:AG8, $P$21:$P$900), 0))</f>
-        <v>#N/A</v>
+        <v>Brossimium alicastrum (Ramon)</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
@@ -11792,58 +11829,58 @@
     <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <f>'PSP Data'!A55</f>
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="B52" t="str">
         <f>IF('PSP Data'!B55=0,"",'PSP Data'!B55)</f>
-        <v/>
-      </c>
-      <c r="C52">
+        <v>Brossimium alicastrum (Ramon)</v>
+      </c>
+      <c r="C52" t="str">
         <f>'PSP Data'!C55</f>
-        <v>0</v>
-      </c>
-      <c r="D52">
+        <v>1O.4</v>
+      </c>
+      <c r="D52" t="str">
         <f>'PSP Data'!E55</f>
-        <v>0</v>
-      </c>
-      <c r="E52">
+        <v>n</v>
+      </c>
+      <c r="E52" t="str">
         <f>'PSP Data'!F55</f>
-        <v>0</v>
-      </c>
-      <c r="F52">
+        <v>y</v>
+      </c>
+      <c r="F52" t="str">
         <f>'PSP Data'!G55</f>
-        <v>0</v>
+        <v>y</v>
       </c>
       <c r="G52">
         <f>'PSP Data'!H55</f>
-        <v>0</v>
+        <v>-88.336830000000006</v>
       </c>
       <c r="H52">
         <f>'PSP Data'!I55</f>
-        <v>0</v>
+        <v>18.03153</v>
       </c>
       <c r="I52">
         <f>'PSP Data'!J55</f>
-        <v>0</v>
-      </c>
-      <c r="J52" s="23" t="e">
+        <v>57.3</v>
+      </c>
+      <c r="J52" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="K52" s="23" t="e">
+        <v>1O.4</v>
+      </c>
+      <c r="K52" s="23" t="str">
         <f>IF(AND((A52&lt;'PSP Data'!$C$11),(A52&lt;&gt;0)),Analysis!C52,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L52" t="e">
+        <v>1O.4</v>
+      </c>
+      <c r="L52" t="str">
         <f>IF(VLOOKUP(B52,Table1[],4)=0,"unknown", VLOOKUP(B52,Table1[],4))</f>
-        <v>#N/A</v>
+        <v>habitat</v>
       </c>
       <c r="M52">
         <v>1</v>
       </c>
-      <c r="N52" t="e">
+      <c r="N52" t="str">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="O52" t="str">
         <f t="shared" si="2"/>
@@ -11851,11 +11888,11 @@
       </c>
       <c r="P52" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Q52" t="str">
+        <v>Brossimium alicastrum (Ramon)</v>
+      </c>
+      <c r="Q52" t="b">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.35">
@@ -70382,8 +70419,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>